<commit_message>
updated totes and feeding
</commit_message>
<xml_diff>
--- a/data/2017-07-30-pacific-oyster-larvae/2017-07-30-Feeding.xlsx
+++ b/data/2017-07-30-pacific-oyster-larvae/2017-07-30-Feeding.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Notes</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Extremely dense, most likely undercounting</t>
+  </si>
+  <si>
+    <t>500 mL Ciso, 250 609, 250 Chagra</t>
+  </si>
+  <si>
+    <t>Extremely dense, most likely undercounting. 15 and 16 accidentally fed 400 mL mix + 100 Chagra + 100 609</t>
   </si>
 </sst>
 </file>
@@ -809,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1097,6 +1103,12 @@
       <c r="E6">
         <v>165</v>
       </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
       <c r="H6">
         <f>AVERAGE(C6:G6)</f>
         <v>168.66666666666666</v>
@@ -1114,18 +1126,71 @@
         <v>444.66403162055332</v>
       </c>
       <c r="L6">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="M6">
         <f>L6*I6</f>
-        <v>759000000</v>
+        <v>843333333.33333337</v>
       </c>
       <c r="N6">
         <f>M6/15000</f>
-        <v>50600</v>
+        <v>56222.222222222226</v>
       </c>
       <c r="O6" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>42951</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>243</v>
+      </c>
+      <c r="D7">
+        <v>231</v>
+      </c>
+      <c r="E7">
+        <v>131</v>
+      </c>
+      <c r="F7">
+        <v>268</v>
+      </c>
+      <c r="G7">
+        <v>159</v>
+      </c>
+      <c r="H7">
+        <f>AVERAGE(C7:G7)</f>
+        <v>206.4</v>
+      </c>
+      <c r="I7">
+        <f>(H7*9)/0.0009</f>
+        <v>2064000.0000000002</v>
+      </c>
+      <c r="J7">
+        <f>15000*50000</f>
+        <v>750000000</v>
+      </c>
+      <c r="K7">
+        <f>J7/I7</f>
+        <v>363.37209302325579</v>
+      </c>
+      <c r="L7">
+        <v>400</v>
+      </c>
+      <c r="M7">
+        <f>L7*I7</f>
+        <v>825600000.00000012</v>
+      </c>
+      <c r="N7">
+        <f>M7/15000</f>
+        <v>55040.000000000007</v>
+      </c>
+      <c r="O7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added feeding and count info
</commit_message>
<xml_diff>
--- a/data/2017-07-30-pacific-oyster-larvae/2017-07-30-Feeding.xlsx
+++ b/data/2017-07-30-pacific-oyster-larvae/2017-07-30-Feeding.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>Notes</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Extremely dense, most likely undercounting. 15 and 16 accidentally fed 400 mL mix + 100 Chagra + 100 609</t>
+  </si>
+  <si>
+    <t>400 mL Ciso, 200 609, 200 Chagra</t>
+  </si>
+  <si>
+    <t>250 mL Ciso, 150 609, 150 Chagra. Concentration must likely an overestimate</t>
   </si>
 </sst>
 </file>
@@ -815,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -905,26 +911,26 @@
         <v>146</v>
       </c>
       <c r="I2">
-        <f>(H2*9)/0.0009</f>
+        <f t="shared" ref="I2:I8" si="0">(H2*9)/0.0009</f>
         <v>1460000</v>
       </c>
       <c r="J2">
-        <f>15000*50000</f>
+        <f t="shared" ref="J2:J8" si="1">15000*50000</f>
         <v>750000000</v>
       </c>
       <c r="K2">
-        <f>J2/I2</f>
+        <f t="shared" ref="K2:K8" si="2">J2/I2</f>
         <v>513.69863013698625</v>
       </c>
       <c r="L2">
         <v>60</v>
       </c>
       <c r="M2">
-        <f>L2*I2</f>
+        <f t="shared" ref="M2:M8" si="3">L2*I2</f>
         <v>87600000</v>
       </c>
       <c r="N2">
-        <f>M2/15000</f>
+        <f t="shared" ref="N2:N8" si="4">M2/15000</f>
         <v>5840</v>
       </c>
       <c r="O2" t="s">
@@ -958,26 +964,26 @@
         <v>129.6</v>
       </c>
       <c r="I3">
-        <f>(H3*9)/0.0009</f>
+        <f t="shared" si="0"/>
         <v>1296000</v>
       </c>
       <c r="J3">
-        <f>15000*50000</f>
+        <f t="shared" si="1"/>
         <v>750000000</v>
       </c>
       <c r="K3">
-        <f>J3/I3</f>
+        <f t="shared" si="2"/>
         <v>578.7037037037037</v>
       </c>
       <c r="L3">
         <v>700</v>
       </c>
       <c r="M3">
-        <f>L3*I3</f>
+        <f t="shared" si="3"/>
         <v>907200000</v>
       </c>
       <c r="N3">
-        <f>M3/15000</f>
+        <f t="shared" si="4"/>
         <v>60480</v>
       </c>
       <c r="O3" t="s">
@@ -1011,26 +1017,26 @@
         <v>41.2</v>
       </c>
       <c r="I4">
-        <f>(H4*9)/0.0009</f>
+        <f t="shared" si="0"/>
         <v>412000</v>
       </c>
       <c r="J4">
-        <f>15000*50000</f>
+        <f t="shared" si="1"/>
         <v>750000000</v>
       </c>
       <c r="K4">
-        <f>J4/I4</f>
+        <f t="shared" si="2"/>
         <v>1820.3883495145631</v>
       </c>
       <c r="L4">
         <v>2100</v>
       </c>
       <c r="M4">
-        <f>L4*I4</f>
+        <f t="shared" si="3"/>
         <v>865200000</v>
       </c>
       <c r="N4">
-        <f>M4/15000</f>
+        <f t="shared" si="4"/>
         <v>57680</v>
       </c>
       <c r="O4" t="s">
@@ -1064,26 +1070,26 @@
         <v>112.2</v>
       </c>
       <c r="I5">
-        <f>(H5*9)/0.0009</f>
+        <f t="shared" si="0"/>
         <v>1122000</v>
       </c>
       <c r="J5">
-        <f>15000*50000</f>
+        <f t="shared" si="1"/>
         <v>750000000</v>
       </c>
       <c r="K5">
-        <f>J5/I5</f>
+        <f t="shared" si="2"/>
         <v>668.44919786096261</v>
       </c>
       <c r="L5">
         <v>700</v>
       </c>
       <c r="M5">
-        <f>L5*I5</f>
+        <f t="shared" si="3"/>
         <v>785400000</v>
       </c>
       <c r="N5">
-        <f>M5/15000</f>
+        <f t="shared" si="4"/>
         <v>52360</v>
       </c>
     </row>
@@ -1114,26 +1120,26 @@
         <v>168.66666666666666</v>
       </c>
       <c r="I6">
-        <f>(H6*9)/0.0009</f>
+        <f t="shared" si="0"/>
         <v>1686666.6666666667</v>
       </c>
       <c r="J6">
-        <f>15000*50000</f>
+        <f t="shared" si="1"/>
         <v>750000000</v>
       </c>
       <c r="K6">
-        <f>J6/I6</f>
+        <f t="shared" si="2"/>
         <v>444.66403162055332</v>
       </c>
       <c r="L6">
         <v>500</v>
       </c>
       <c r="M6">
-        <f>L6*I6</f>
+        <f t="shared" si="3"/>
         <v>843333333.33333337</v>
       </c>
       <c r="N6">
-        <f>M6/15000</f>
+        <f t="shared" si="4"/>
         <v>56222.222222222226</v>
       </c>
       <c r="O6" t="s">
@@ -1167,30 +1173,83 @@
         <v>206.4</v>
       </c>
       <c r="I7">
-        <f>(H7*9)/0.0009</f>
+        <f t="shared" si="0"/>
         <v>2064000.0000000002</v>
       </c>
       <c r="J7">
-        <f>15000*50000</f>
+        <f t="shared" si="1"/>
         <v>750000000</v>
       </c>
       <c r="K7">
-        <f>J7/I7</f>
+        <f t="shared" si="2"/>
         <v>363.37209302325579</v>
       </c>
       <c r="L7">
         <v>400</v>
       </c>
       <c r="M7">
-        <f>L7*I7</f>
+        <f t="shared" si="3"/>
         <v>825600000.00000012</v>
       </c>
       <c r="N7">
-        <f>M7/15000</f>
+        <f t="shared" si="4"/>
         <v>55040.000000000007</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>42952</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>195</v>
+      </c>
+      <c r="D8">
+        <v>215</v>
+      </c>
+      <c r="E8">
+        <v>290</v>
+      </c>
+      <c r="F8">
+        <v>216</v>
+      </c>
+      <c r="G8">
+        <v>238</v>
+      </c>
+      <c r="H8">
+        <f>AVERAGE(C8:G8)</f>
+        <v>230.8</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>2308000.0000000005</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>750000000</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>324.95667244367411</v>
+      </c>
+      <c r="L8">
+        <v>550</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>1269400000.0000002</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>84626.666666666686</v>
+      </c>
+      <c r="O8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added feeding information from 8/6
</commit_message>
<xml_diff>
--- a/data/2017-07-30-pacific-oyster-larvae/2017-07-30-Feeding.xlsx
+++ b/data/2017-07-30-pacific-oyster-larvae/2017-07-30-Feeding.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Notes</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>250 mL Ciso, 150 609, 150 Chagra. Concentration must likely an overestimate</t>
+  </si>
+  <si>
+    <t>250 mL Ciso, 125 609, 125 Chagra. Extremely dense, most likely undercounting</t>
   </si>
 </sst>
 </file>
@@ -822,7 +825,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -911,26 +914,26 @@
         <v>146</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I8" si="0">(H2*9)/0.0009</f>
+        <f t="shared" ref="I2:I9" si="0">(H2*9)/0.0009</f>
         <v>1460000</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J8" si="1">15000*50000</f>
+        <f t="shared" ref="J2:J9" si="1">15000*50000</f>
         <v>750000000</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K8" si="2">J2/I2</f>
+        <f t="shared" ref="K2:K9" si="2">J2/I2</f>
         <v>513.69863013698625</v>
       </c>
       <c r="L2">
         <v>60</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M8" si="3">L2*I2</f>
+        <f t="shared" ref="M2:M9" si="3">L2*I2</f>
         <v>87600000</v>
       </c>
       <c r="N2">
-        <f t="shared" ref="N2:N8" si="4">M2/15000</f>
+        <f t="shared" ref="N2:N9" si="4">M2/15000</f>
         <v>5840</v>
       </c>
       <c r="O2" t="s">
@@ -960,7 +963,7 @@
         <v>161</v>
       </c>
       <c r="H3">
-        <f>AVERAGE(C3:G3)</f>
+        <f t="shared" ref="H3:H9" si="5">AVERAGE(C3:G3)</f>
         <v>129.6</v>
       </c>
       <c r="I3">
@@ -1013,7 +1016,7 @@
         <v>49</v>
       </c>
       <c r="H4">
-        <f>AVERAGE(C4:G4)</f>
+        <f t="shared" si="5"/>
         <v>41.2</v>
       </c>
       <c r="I4">
@@ -1066,7 +1069,7 @@
         <v>130</v>
       </c>
       <c r="H5">
-        <f>AVERAGE(C5:G5)</f>
+        <f t="shared" si="5"/>
         <v>112.2</v>
       </c>
       <c r="I5">
@@ -1116,7 +1119,7 @@
         <v>15</v>
       </c>
       <c r="H6">
-        <f>AVERAGE(C6:G6)</f>
+        <f t="shared" si="5"/>
         <v>168.66666666666666</v>
       </c>
       <c r="I6">
@@ -1169,7 +1172,7 @@
         <v>159</v>
       </c>
       <c r="H7">
-        <f>AVERAGE(C7:G7)</f>
+        <f t="shared" si="5"/>
         <v>206.4</v>
       </c>
       <c r="I7">
@@ -1222,7 +1225,7 @@
         <v>238</v>
       </c>
       <c r="H8">
-        <f>AVERAGE(C8:G8)</f>
+        <f t="shared" si="5"/>
         <v>230.8</v>
       </c>
       <c r="I8">
@@ -1250,6 +1253,59 @@
       </c>
       <c r="O8" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>42953</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>252</v>
+      </c>
+      <c r="D9">
+        <v>181</v>
+      </c>
+      <c r="E9">
+        <v>197</v>
+      </c>
+      <c r="F9">
+        <v>214</v>
+      </c>
+      <c r="G9">
+        <v>221</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="5"/>
+        <v>213</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>2130000</v>
+      </c>
+      <c r="J9">
+        <f>15000*65000</f>
+        <v>975000000</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>457.74647887323943</v>
+      </c>
+      <c r="L9">
+        <v>500</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>1065000000</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>71000</v>
+      </c>
+      <c r="O9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated tote positions, feeding log and larval counts
</commit_message>
<xml_diff>
--- a/data/2017-07-30-pacific-oyster-larvae/2017-07-30-Feeding.xlsx
+++ b/data/2017-07-30-pacific-oyster-larvae/2017-07-30-Feeding.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Notes</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>250 mL Ciso, 125 609, 125 Chagra. Extremely dense, most likely undercounting</t>
+  </si>
+  <si>
+    <t>Extremely dense. 150 mL Ciso, 75 mL 609, 75 mL Chagra</t>
   </si>
 </sst>
 </file>
@@ -824,9 +827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
-    </sheetView>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -918,7 +919,7 @@
         <v>1460000</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J9" si="1">15000*50000</f>
+        <f t="shared" ref="J2:J8" si="1">15000*50000</f>
         <v>750000000</v>
       </c>
       <c r="K2">
@@ -929,11 +930,11 @@
         <v>60</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M9" si="3">L2*I2</f>
+        <f t="shared" ref="M2:M10" si="3">L2*I2</f>
         <v>87600000</v>
       </c>
       <c r="N2">
-        <f t="shared" ref="N2:N9" si="4">M2/15000</f>
+        <f t="shared" ref="N2:N10" si="4">M2/15000</f>
         <v>5840</v>
       </c>
       <c r="O2" t="s">
@@ -963,7 +964,7 @@
         <v>161</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H9" si="5">AVERAGE(C3:G3)</f>
+        <f t="shared" ref="H3:H10" si="5">AVERAGE(C3:G3)</f>
         <v>129.6</v>
       </c>
       <c r="I3">
@@ -1306,6 +1307,59 @@
       </c>
       <c r="O9" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>42954</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>340</v>
+      </c>
+      <c r="D10">
+        <v>360</v>
+      </c>
+      <c r="E10">
+        <v>320</v>
+      </c>
+      <c r="F10">
+        <v>365</v>
+      </c>
+      <c r="G10">
+        <v>299</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="5"/>
+        <v>336.8</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ref="I10" si="6">(H10*9)/0.0009</f>
+        <v>3368000.0000000005</v>
+      </c>
+      <c r="J10">
+        <f>15000*65000</f>
+        <v>975000000</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10" si="7">J10/I10</f>
+        <v>289.48931116389542</v>
+      </c>
+      <c r="L10">
+        <v>300</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>1010400000.0000001</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>67360.000000000015</v>
+      </c>
+      <c r="O10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>